<commit_message>
Read and write file excel
</commit_message>
<xml_diff>
--- a/example_with_multiple_tables.xlsx
+++ b/example_with_multiple_tables.xlsx
@@ -8,12 +8,16 @@
   <sheets>
     <sheet name="Anken List" r:id="rId3" sheetId="1"/>
     <sheet name="Category_Account" r:id="rId4" sheetId="2"/>
+    <sheet name="Category_Campaign" r:id="rId5" sheetId="3"/>
   </sheets>
+  <definedNames>
+    <definedName name="AnkenList">Anken List!$B$2:$B$71</definedName>
+  </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="69">
   <si>
     <t>Anken Id</t>
   </si>
@@ -169,6 +173,57 @@
   </si>
   <si>
     <t>Category 4</t>
+  </si>
+  <si>
+    <t>Campaign Code</t>
+  </si>
+  <si>
+    <t>Campaign Id</t>
+  </si>
+  <si>
+    <t>Campaign Name</t>
+  </si>
+  <si>
+    <t>AD Update</t>
+  </si>
+  <si>
+    <t>Campaign 1</t>
+  </si>
+  <si>
+    <t>aaaa</t>
+  </si>
+  <si>
+    <t>Campaign 2</t>
+  </si>
+  <si>
+    <t>New Category</t>
+  </si>
+  <si>
+    <t>Campaign 3</t>
+  </si>
+  <si>
+    <t>Campaign 4</t>
+  </si>
+  <si>
+    <t>Campaign 5</t>
+  </si>
+  <si>
+    <t>Campaign 6</t>
+  </si>
+  <si>
+    <t>Campaign 7</t>
+  </si>
+  <si>
+    <t>Campaign 8</t>
+  </si>
+  <si>
+    <t>Campaign 9</t>
+  </si>
+  <si>
+    <t>Campaign 10</t>
+  </si>
+  <si>
+    <t>Campaign 11</t>
   </si>
 </sst>
 </file>
@@ -207,8 +262,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
@@ -821,6 +877,482 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" sqref="A2:A15" allowBlank="true" errorStyle="stop">
+      <formula1>AnkenList</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="I2:I15" allowBlank="true" errorStyle="stop">
+      <formula1>"Update,Delete,None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="R2:R6" allowBlank="true" errorStyle="stop">
+      <formula1>"Update,Delete,None"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:T12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>45607.0</v>
+      </c>
+      <c r="H2" t="n" s="2">
+        <v>45607.0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>56</v>
+      </c>
+      <c r="R2" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="S2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>45607.0</v>
+      </c>
+      <c r="H3" t="n" s="2">
+        <v>45607.0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S3"/>
+      <c r="T3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>26.0</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="S4" t="s">
+        <v>55</v>
+      </c>
+      <c r="T4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="K5" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="L5" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="M5" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="N5" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="O5" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="P5" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="Q5" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="S5" s="0"/>
+      <c r="T5" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="K6" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="L6" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="M6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="N6" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="O6" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="P6" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="Q6" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="S6" s="0"/>
+      <c r="T6" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="K7" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="L7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="M7" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="N7" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="O7" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="P7" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="Q7" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="S7" s="0"/>
+      <c r="T7" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="K8" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="L8" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="M8" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="N8" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="O8" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="P8" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="Q8" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="S8" s="0"/>
+      <c r="T8" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="K9" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="L9" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="M9" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="N9" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="O9" t="n" s="0">
+        <v>8.0</v>
+      </c>
+      <c r="P9" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="Q9" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="S9" s="0"/>
+      <c r="T9" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="K10" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="L10" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="M10" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="N10" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="O10" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="P10" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="Q10" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="S10" s="0"/>
+      <c r="T10" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="K11" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="L11" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="M11" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="N11" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="O11" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="P11" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="Q11" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="S11" s="0"/>
+      <c r="T11" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="K12" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="L12" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="M12" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="N12" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="O12" t="n" s="0">
+        <v>11.0</v>
+      </c>
+      <c r="P12" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="Q12" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="S12" s="0"/>
+      <c r="T12" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" sqref="A2:A4" allowBlank="true" errorStyle="stop">
+      <formula1>AnkenList</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="I2:I4" allowBlank="true" errorStyle="stop">
+      <formula1>"Update,Delete,None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="T2:T12" allowBlank="true" errorStyle="stop">
+      <formula1>"Update,Delete,None"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completed basic work with file excel
</commit_message>
<xml_diff>
--- a/example_with_multiple_tables.xlsx
+++ b/example_with_multiple_tables.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="70">
   <si>
     <t>Anken Id</t>
   </si>
@@ -82,7 +82,7 @@
     <t>Account Code</t>
   </si>
   <si>
-    <t>b</t>
+    <t>ab</t>
   </si>
   <si>
     <t/>
@@ -103,7 +103,7 @@
     <t>Category 6</t>
   </si>
   <si>
-    <t>ab</t>
+    <t>abc</t>
   </si>
   <si>
     <t>Account 2 - FB</t>
@@ -115,7 +115,10 @@
     <t>Category3</t>
   </si>
   <si>
-    <t>abc</t>
+    <t>e</t>
+  </si>
+  <si>
+    <t>IMP</t>
   </si>
   <si>
     <t>Account 3 - GG</t>
@@ -127,10 +130,7 @@
     <t>GG</t>
   </si>
   <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>IMP</t>
+    <t>eo</t>
   </si>
   <si>
     <t>Account 4 - Yahho</t>
@@ -142,7 +142,13 @@
     <t>YAH</t>
   </si>
   <si>
-    <t>eo</t>
+    <t>qwere</t>
+  </si>
+  <si>
+    <t>adv</t>
+  </si>
+  <si>
+    <t>CPC</t>
   </si>
   <si>
     <t>Account 5- GG</t>
@@ -151,12 +157,6 @@
     <t>ACC_5</t>
   </si>
   <si>
-    <t>adv</t>
-  </si>
-  <si>
-    <t>CPC</t>
-  </si>
-  <si>
     <t>AD</t>
   </si>
   <si>
@@ -166,7 +166,10 @@
     <t>qwer</t>
   </si>
   <si>
-    <t>qwere</t>
+    <t>Category Update</t>
+  </si>
+  <si>
+    <t>qweree</t>
   </si>
   <si>
     <t>Category1</t>
@@ -190,13 +193,13 @@
     <t>Campaign 1</t>
   </si>
   <si>
-    <t>aaaa</t>
+    <t>New Category</t>
   </si>
   <si>
     <t>Campaign 2</t>
   </si>
   <si>
-    <t>New Category</t>
+    <t>Tesst</t>
   </si>
   <si>
     <t>Campaign 3</t>
@@ -349,7 +352,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -413,7 +416,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>21</v>
@@ -460,13 +463,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>28</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>0.0</v>
+        <v>10000.0</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>22</v>
@@ -506,20 +509,26 @@
       <c r="A4" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B4" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="C4" t="s" s="0">
+      <c r="B4" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="n" s="0">
-        <v>10000.0</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>22</v>
+      <c r="D4" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
       </c>
       <c r="F4" t="n">
         <v>0.0</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>45515.0</v>
+      </c>
+      <c r="H4" t="n" s="1">
+        <v>45524.0</v>
       </c>
       <c r="I4" t="s">
         <v>23</v>
@@ -531,13 +540,13 @@
         <v>3.0</v>
       </c>
       <c r="M4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q4"/>
       <c r="R4" t="s">
@@ -548,26 +557,20 @@
       <c r="A5" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B5" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" t="n">
+      <c r="B5" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D5" t="n" s="0">
         <v>100000.0</v>
       </c>
-      <c r="E5" t="s">
-        <v>37</v>
+      <c r="E5" t="s" s="0">
+        <v>33</v>
       </c>
       <c r="F5" t="n">
         <v>0.0</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>45515.0</v>
-      </c>
-      <c r="H5" t="n" s="1">
-        <v>45524.0</v>
       </c>
       <c r="I5" t="s">
         <v>23</v>
@@ -587,7 +590,12 @@
       <c r="O5" t="s">
         <v>40</v>
       </c>
-      <c r="Q5"/>
+      <c r="P5" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>41</v>
+      </c>
       <c r="R5" t="s">
         <v>23</v>
       </c>
@@ -596,20 +604,26 @@
       <c r="A6" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B6" t="n" s="0">
-        <v>6.0</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="D6" t="n" s="0">
-        <v>100000.0</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>37</v>
+      <c r="B6" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
       </c>
       <c r="F6" t="n">
         <v>0.0</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>45607.0</v>
+      </c>
+      <c r="H6" t="n" s="1">
+        <v>45607.0</v>
       </c>
       <c r="I6" t="s">
         <v>23</v>
@@ -621,13 +635,13 @@
         <v>5.0</v>
       </c>
       <c r="M6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="O6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P6" t="n">
         <v>25.0</v>
@@ -644,16 +658,16 @@
         <v>2</v>
       </c>
       <c r="B7" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D7" t="n">
         <v>0.0</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F7" t="n">
         <v>0.0</v>
@@ -672,26 +686,20 @@
       <c r="A8" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B8" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>45</v>
+      <c r="B8" t="n" s="0">
+        <v>14.0</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="D8" t="n" s="0">
+        <v>100000.0</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>33</v>
       </c>
       <c r="F8" t="n">
         <v>0.0</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>45607.0</v>
-      </c>
-      <c r="H8" t="n" s="1">
-        <v>45607.0</v>
       </c>
       <c r="I8" t="s">
         <v>23</v>
@@ -702,16 +710,16 @@
         <v>2</v>
       </c>
       <c r="B9" t="n" s="0">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D9" t="n" s="0">
         <v>100000.0</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F9" t="n">
         <v>0.0</v>
@@ -725,16 +733,16 @@
         <v>2</v>
       </c>
       <c r="B10" t="n" s="0">
-        <v>15.0</v>
+        <v>17.0</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D10" t="n" s="0">
         <v>100000.0</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F10" t="n">
         <v>0.0</v>
@@ -748,7 +756,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="n" s="0">
-        <v>17.0</v>
+        <v>27.0</v>
       </c>
       <c r="C11" t="s" s="0">
         <v>49</v>
@@ -757,7 +765,7 @@
         <v>100000.0</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F11" t="n">
         <v>0.0</v>
@@ -768,28 +776,22 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="B12" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="n" s="0">
+        <v>29.0</v>
+      </c>
+      <c r="C12" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="D12" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>45</v>
+      <c r="D12" t="n" s="0">
+        <v>100000.0</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>33</v>
       </c>
       <c r="F12" t="n">
         <v>0.0</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>45607.0</v>
-      </c>
-      <c r="H12" t="n" s="1">
-        <v>45607.0</v>
       </c>
       <c r="I12" t="s">
         <v>23</v>
@@ -799,20 +801,26 @@
       <c r="A13" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B13" t="n" s="0">
-        <v>25.0</v>
-      </c>
-      <c r="C13" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="D13" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E13" t="s" s="0">
-        <v>37</v>
+      <c r="B13" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
       </c>
       <c r="F13" t="n">
         <v>0.0</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>45607.0</v>
+      </c>
+      <c r="H13" t="n" s="1">
+        <v>45607.0</v>
       </c>
       <c r="I13" t="s">
         <v>23</v>
@@ -820,28 +828,22 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="B14" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="n">
-        <v>10000.0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>37</v>
+        <v>3</v>
+      </c>
+      <c r="B14" t="n" s="0">
+        <v>25.0</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>33</v>
       </c>
       <c r="F14" t="n">
         <v>0.0</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>45607.0</v>
-      </c>
-      <c r="H14" t="n" s="1">
-        <v>45607.0</v>
       </c>
       <c r="I14" t="s">
         <v>23</v>
@@ -852,36 +854,65 @@
         <v>8</v>
       </c>
       <c r="B15" t="n">
-        <v>23.0</v>
+        <v>22.0</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="D15" t="n">
         <v>10000.0</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F15" t="n">
         <v>0.0</v>
       </c>
       <c r="G15" s="1" t="n">
+        <v>45607.0</v>
+      </c>
+      <c r="H15" t="n" s="1">
+        <v>45607.0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B16" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G16" s="1" t="n">
         <v>45617.0</v>
       </c>
-      <c r="H15" t="n" s="1">
+      <c r="H16" t="n" s="1">
         <v>45617.0</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I16" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" sqref="A2:A15" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="A2:A16" allowBlank="true" errorStyle="stop">
       <formula1>AnkenList</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="I2:I15" allowBlank="true" errorStyle="stop">
+    <dataValidation type="list" sqref="I2:I16" allowBlank="true" errorStyle="stop">
       <formula1>"Update,Delete,None"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="R2:R6" allowBlank="true" errorStyle="stop">
@@ -941,13 +972,13 @@
         <v>19</v>
       </c>
       <c r="O1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" t="s">
         <v>53</v>
-      </c>
-      <c r="P1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>52</v>
       </c>
       <c r="R1" t="s">
         <v>15</v>
@@ -967,13 +998,13 @@
         <v>9.0</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D2" t="n">
         <v>0.0</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F2" t="n">
         <v>0.0</v>
@@ -1003,10 +1034,10 @@
         <v>1.0</v>
       </c>
       <c r="P2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="R2" t="n">
         <v>22.0</v>
@@ -1022,26 +1053,20 @@
       <c r="A3" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>45</v>
+      <c r="B3" t="n" s="0">
+        <v>26.0</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>33</v>
       </c>
       <c r="F3" t="n">
         <v>0.0</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>45607.0</v>
-      </c>
-      <c r="H3" t="n" s="2">
-        <v>45607.0</v>
       </c>
       <c r="I3" t="s">
         <v>23</v>
@@ -1062,34 +1087,45 @@
         <v>2.0</v>
       </c>
       <c r="P3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>59</v>
+      </c>
+      <c r="R3" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="S3" t="s">
         <v>58</v>
       </c>
-      <c r="Q3" t="s">
-        <v>58</v>
-      </c>
-      <c r="S3"/>
       <c r="T3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n" s="0">
-        <v>26.0</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>59</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>37</v>
+        <v>5</v>
+      </c>
+      <c r="B4" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
       </c>
       <c r="F4" t="n">
         <v>0.0</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>45621.0</v>
+      </c>
+      <c r="H4" t="n" s="2">
+        <v>45621.0</v>
       </c>
       <c r="I4" t="s">
         <v>23</v>
@@ -1110,16 +1146,16 @@
         <v>3.0</v>
       </c>
       <c r="P4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="R4" t="n">
         <v>9.0</v>
       </c>
       <c r="S4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="T4" t="s">
         <v>23</v>
@@ -1142,10 +1178,10 @@
         <v>4.0</v>
       </c>
       <c r="P5" t="s" s="0">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q5" t="s" s="0">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S5" s="0"/>
       <c r="T5" t="s" s="0">
@@ -1169,10 +1205,10 @@
         <v>5.0</v>
       </c>
       <c r="P6" t="s" s="0">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Q6" t="s" s="0">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="S6" s="0"/>
       <c r="T6" t="s" s="0">
@@ -1184,22 +1220,22 @@
         <v>3</v>
       </c>
       <c r="L7" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M7" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N7" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O7" t="n" s="0">
         <v>6.0</v>
       </c>
       <c r="P7" t="s" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="Q7" t="s" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="S7" s="0"/>
       <c r="T7" t="s" s="0">
@@ -1211,22 +1247,22 @@
         <v>3</v>
       </c>
       <c r="L8" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M8" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N8" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O8" t="n" s="0">
         <v>7.0</v>
       </c>
       <c r="P8" t="s" s="0">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Q8" t="s" s="0">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="S8" s="0"/>
       <c r="T8" t="s" s="0">
@@ -1250,10 +1286,10 @@
         <v>8.0</v>
       </c>
       <c r="P9" t="s" s="0">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q9" t="s" s="0">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S9" s="0"/>
       <c r="T9" t="s" s="0">
@@ -1277,10 +1313,10 @@
         <v>9.0</v>
       </c>
       <c r="P10" t="s" s="0">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Q10" t="s" s="0">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="S10" s="0"/>
       <c r="T10" t="s" s="0">
@@ -1292,22 +1328,22 @@
         <v>4</v>
       </c>
       <c r="L11" t="s" s="0">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M11" t="s" s="0">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N11" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O11" t="n" s="0">
         <v>10.0</v>
       </c>
       <c r="P11" t="s" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q11" t="s" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S11" s="0"/>
       <c r="T11" t="s" s="0">
@@ -1319,22 +1355,22 @@
         <v>4</v>
       </c>
       <c r="L12" t="s" s="0">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M12" t="s" s="0">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N12" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O12" t="n" s="0">
         <v>11.0</v>
       </c>
       <c r="P12" t="s" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Q12" t="s" s="0">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="S12" s="0"/>
       <c r="T12" t="s" s="0">

</xml_diff>